<commit_message>
them chuc nang chup anh man hinh
</commit_message>
<xml_diff>
--- a/log_message/ban_tin_da_gui.xlsx
+++ b/log_message/ban_tin_da_gui.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="35">
   <si>
     <t>Thời gian gửi</t>
   </si>
@@ -82,6 +82,30 @@
     <t>4G-TTT072S-HNI</t>
   </si>
   <si>
+    <t>UL_TTT038M_HNI</t>
+  </si>
+  <si>
+    <t>SR_TTT014M_HNI</t>
+  </si>
+  <si>
+    <t>2G_BVI015M_HNI</t>
+  </si>
+  <si>
+    <t>3G_BVI015M_HNI</t>
+  </si>
+  <si>
+    <t>UL_TTT111M_HNI</t>
+  </si>
+  <si>
+    <t>3G_STY030M_HNI</t>
+  </si>
+  <si>
+    <t>2G_STY030M_HNI</t>
+  </si>
+  <si>
+    <t>4G_STY022M_HNI</t>
+  </si>
+  <si>
     <t>SITE_OOS_BY_POWER</t>
   </si>
   <si>
@@ -89,6 +113,9 @@
   </si>
   <si>
     <t>SITE_OOS</t>
+  </si>
+  <si>
+    <t>CELL_OOS, HW_OUTDOOR, HW_TTS_MUC_TRAM</t>
   </si>
   <si>
     <t>Thành công</t>
@@ -453,7 +480,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D120"/>
+  <dimension ref="A1:D129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -481,10 +508,10 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -495,10 +522,10 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -509,10 +536,10 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -523,10 +550,10 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -537,10 +564,10 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -551,10 +578,10 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -565,10 +592,10 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -579,10 +606,10 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -593,10 +620,10 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -607,10 +634,10 @@
         <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -621,10 +648,10 @@
         <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -635,10 +662,10 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -649,10 +676,10 @@
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -663,10 +690,10 @@
         <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D15" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -677,10 +704,10 @@
         <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -691,10 +718,10 @@
         <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -705,10 +732,10 @@
         <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -719,10 +746,10 @@
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -733,10 +760,10 @@
         <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D20" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -747,10 +774,10 @@
         <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D21" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -761,10 +788,10 @@
         <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D22" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -775,10 +802,10 @@
         <v>11</v>
       </c>
       <c r="C23" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D23" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -789,10 +816,10 @@
         <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D24" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -803,10 +830,10 @@
         <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D25" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -817,10 +844,10 @@
         <v>13</v>
       </c>
       <c r="C26" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D26" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -831,10 +858,10 @@
         <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D27" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -845,10 +872,10 @@
         <v>14</v>
       </c>
       <c r="C28" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D28" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -859,10 +886,10 @@
         <v>11</v>
       </c>
       <c r="C29" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D29" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -873,10 +900,10 @@
         <v>9</v>
       </c>
       <c r="C30" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D30" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -887,10 +914,10 @@
         <v>6</v>
       </c>
       <c r="C31" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -901,10 +928,10 @@
         <v>17</v>
       </c>
       <c r="C32" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D32" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -915,10 +942,10 @@
         <v>17</v>
       </c>
       <c r="C33" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D33" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -929,10 +956,10 @@
         <v>7</v>
       </c>
       <c r="C34" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D34" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -943,10 +970,10 @@
         <v>8</v>
       </c>
       <c r="C35" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D35" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -957,10 +984,10 @@
         <v>9</v>
       </c>
       <c r="C36" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D36" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -971,10 +998,10 @@
         <v>18</v>
       </c>
       <c r="C37" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D37" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -985,10 +1012,10 @@
         <v>17</v>
       </c>
       <c r="C38" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D38" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -999,10 +1026,10 @@
         <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D39" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1013,10 +1040,10 @@
         <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D40" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1027,10 +1054,10 @@
         <v>6</v>
       </c>
       <c r="C41" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D41" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1041,10 +1068,10 @@
         <v>19</v>
       </c>
       <c r="C42" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D42" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1055,10 +1082,10 @@
         <v>20</v>
       </c>
       <c r="C43" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D43" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1069,10 +1096,10 @@
         <v>12</v>
       </c>
       <c r="C44" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D44" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1083,10 +1110,10 @@
         <v>13</v>
       </c>
       <c r="C45" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D45" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1097,10 +1124,10 @@
         <v>10</v>
       </c>
       <c r="C46" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D46" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1111,10 +1138,10 @@
         <v>7</v>
       </c>
       <c r="C47" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D47" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1125,10 +1152,10 @@
         <v>8</v>
       </c>
       <c r="C48" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D48" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1139,10 +1166,10 @@
         <v>9</v>
       </c>
       <c r="C49" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D49" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1153,10 +1180,10 @@
         <v>4</v>
       </c>
       <c r="C50" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D50" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1167,10 +1194,10 @@
         <v>5</v>
       </c>
       <c r="C51" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D51" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -1181,10 +1208,10 @@
         <v>6</v>
       </c>
       <c r="C52" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D52" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -1195,10 +1222,10 @@
         <v>17</v>
       </c>
       <c r="C53" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D53" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -1209,10 +1236,10 @@
         <v>17</v>
       </c>
       <c r="C54" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D54" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1223,10 +1250,10 @@
         <v>18</v>
       </c>
       <c r="C55" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D55" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1237,10 +1264,10 @@
         <v>17</v>
       </c>
       <c r="C56" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D56" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -1251,10 +1278,10 @@
         <v>19</v>
       </c>
       <c r="C57" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D57" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -1265,10 +1292,10 @@
         <v>20</v>
       </c>
       <c r="C58" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D58" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -1279,10 +1306,10 @@
         <v>12</v>
       </c>
       <c r="C59" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D59" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -1293,10 +1320,10 @@
         <v>13</v>
       </c>
       <c r="C60" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D60" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -1307,10 +1334,10 @@
         <v>10</v>
       </c>
       <c r="C61" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D61" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1321,10 +1348,10 @@
         <v>7</v>
       </c>
       <c r="C62" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D62" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -1335,10 +1362,10 @@
         <v>8</v>
       </c>
       <c r="C63" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D63" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -1349,10 +1376,10 @@
         <v>9</v>
       </c>
       <c r="C64" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D64" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -1363,10 +1390,10 @@
         <v>4</v>
       </c>
       <c r="C65" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D65" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1377,10 +1404,10 @@
         <v>5</v>
       </c>
       <c r="C66" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D66" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -1391,10 +1418,10 @@
         <v>6</v>
       </c>
       <c r="C67" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D67" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -1405,10 +1432,10 @@
         <v>17</v>
       </c>
       <c r="C68" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D68" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -1419,10 +1446,10 @@
         <v>17</v>
       </c>
       <c r="C69" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D69" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -1433,10 +1460,10 @@
         <v>7</v>
       </c>
       <c r="C70" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D70" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -1447,10 +1474,10 @@
         <v>8</v>
       </c>
       <c r="C71" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D71" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -1461,10 +1488,10 @@
         <v>9</v>
       </c>
       <c r="C72" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D72" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -1475,10 +1502,10 @@
         <v>18</v>
       </c>
       <c r="C73" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D73" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -1489,10 +1516,10 @@
         <v>17</v>
       </c>
       <c r="C74" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D74" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -1503,10 +1530,10 @@
         <v>4</v>
       </c>
       <c r="C75" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D75" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -1517,10 +1544,10 @@
         <v>5</v>
       </c>
       <c r="C76" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D76" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -1531,10 +1558,10 @@
         <v>6</v>
       </c>
       <c r="C77" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D77" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -1545,10 +1572,10 @@
         <v>19</v>
       </c>
       <c r="C78" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D78" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -1559,10 +1586,10 @@
         <v>20</v>
       </c>
       <c r="C79" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D79" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -1573,10 +1600,10 @@
         <v>12</v>
       </c>
       <c r="C80" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D80" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -1587,10 +1614,10 @@
         <v>13</v>
       </c>
       <c r="C81" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D81" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -1601,10 +1628,10 @@
         <v>10</v>
       </c>
       <c r="C82" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D82" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -1615,10 +1642,10 @@
         <v>21</v>
       </c>
       <c r="C83" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="D83" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -1629,10 +1656,10 @@
         <v>4</v>
       </c>
       <c r="C84" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D84" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -1643,10 +1670,10 @@
         <v>5</v>
       </c>
       <c r="C85" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D85" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -1657,10 +1684,10 @@
         <v>6</v>
       </c>
       <c r="C86" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D86" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -1671,10 +1698,10 @@
         <v>7</v>
       </c>
       <c r="C87" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D87" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -1685,10 +1712,10 @@
         <v>8</v>
       </c>
       <c r="C88" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D88" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -1699,10 +1726,10 @@
         <v>9</v>
       </c>
       <c r="C89" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D89" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -1713,10 +1740,10 @@
         <v>17</v>
       </c>
       <c r="C90" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D90" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -1727,10 +1754,10 @@
         <v>17</v>
       </c>
       <c r="C91" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D91" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -1741,10 +1768,10 @@
         <v>18</v>
       </c>
       <c r="C92" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D92" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -1755,10 +1782,10 @@
         <v>17</v>
       </c>
       <c r="C93" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D93" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -1769,10 +1796,10 @@
         <v>19</v>
       </c>
       <c r="C94" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D94" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -1783,10 +1810,10 @@
         <v>20</v>
       </c>
       <c r="C95" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D95" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -1797,10 +1824,10 @@
         <v>12</v>
       </c>
       <c r="C96" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D96" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -1811,10 +1838,10 @@
         <v>13</v>
       </c>
       <c r="C97" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D97" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -1825,10 +1852,10 @@
         <v>7</v>
       </c>
       <c r="C98" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D98" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -1839,10 +1866,10 @@
         <v>8</v>
       </c>
       <c r="C99" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D99" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -1853,10 +1880,10 @@
         <v>9</v>
       </c>
       <c r="C100" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D100" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -1867,10 +1894,10 @@
         <v>4</v>
       </c>
       <c r="C101" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D101" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -1881,10 +1908,10 @@
         <v>5</v>
       </c>
       <c r="C102" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D102" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -1895,10 +1922,10 @@
         <v>6</v>
       </c>
       <c r="C103" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D103" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -1909,10 +1936,10 @@
         <v>17</v>
       </c>
       <c r="C104" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D104" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -1923,10 +1950,10 @@
         <v>17</v>
       </c>
       <c r="C105" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D105" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -1937,10 +1964,10 @@
         <v>7</v>
       </c>
       <c r="C106" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D106" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -1951,10 +1978,10 @@
         <v>8</v>
       </c>
       <c r="C107" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D107" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -1965,10 +1992,10 @@
         <v>9</v>
       </c>
       <c r="C108" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D108" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -1979,10 +2006,10 @@
         <v>18</v>
       </c>
       <c r="C109" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D109" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -1993,10 +2020,10 @@
         <v>17</v>
       </c>
       <c r="C110" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D110" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -2007,10 +2034,10 @@
         <v>4</v>
       </c>
       <c r="C111" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D111" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -2021,10 +2048,10 @@
         <v>5</v>
       </c>
       <c r="C112" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D112" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -2035,10 +2062,10 @@
         <v>6</v>
       </c>
       <c r="C113" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D113" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -2049,10 +2076,10 @@
         <v>19</v>
       </c>
       <c r="C114" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D114" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -2063,80 +2090,206 @@
         <v>20</v>
       </c>
       <c r="C115" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D115" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="2">
-        <v>45754.73332535636</v>
+        <v>45754.73332535879</v>
       </c>
       <c r="B116" t="s">
         <v>12</v>
       </c>
       <c r="C116" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D116" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="2">
-        <v>45754.73333599294</v>
+        <v>45754.73333599537</v>
       </c>
       <c r="B117" t="s">
         <v>13</v>
       </c>
       <c r="C117" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D117" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="2">
-        <v>45754.73334625367</v>
+        <v>45754.73334625</v>
       </c>
       <c r="B118" t="s">
         <v>10</v>
       </c>
       <c r="C118" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D118" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="2">
-        <v>45754.73335609154</v>
+        <v>45754.73335608796</v>
       </c>
       <c r="B119" t="s">
         <v>14</v>
       </c>
       <c r="C119" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D119" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="2">
-        <v>45754.73336722183</v>
+        <v>45754.73336722222</v>
       </c>
       <c r="B120" t="s">
         <v>11</v>
       </c>
       <c r="C120" t="s">
+        <v>31</v>
+      </c>
+      <c r="D120" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" s="2">
+        <v>45755.34974707176</v>
+      </c>
+      <c r="B121" t="s">
+        <v>19</v>
+      </c>
+      <c r="C121" t="s">
+        <v>31</v>
+      </c>
+      <c r="D121" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122" s="2">
+        <v>45755.36286347222</v>
+      </c>
+      <c r="B122" t="s">
+        <v>22</v>
+      </c>
+      <c r="C122" t="s">
+        <v>31</v>
+      </c>
+      <c r="D122" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123" s="2">
+        <v>45755.41738707176</v>
+      </c>
+      <c r="B123" t="s">
         <v>23</v>
       </c>
-      <c r="D120" t="s">
+      <c r="C123" t="s">
+        <v>31</v>
+      </c>
+      <c r="D123" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124" s="2">
+        <v>45755.42811016204</v>
+      </c>
+      <c r="B124" t="s">
+        <v>24</v>
+      </c>
+      <c r="C124" t="s">
+        <v>32</v>
+      </c>
+      <c r="D124" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125" s="2">
+        <v>45755.42812280093</v>
+      </c>
+      <c r="B125" t="s">
         <v>25</v>
+      </c>
+      <c r="C125" t="s">
+        <v>32</v>
+      </c>
+      <c r="D125" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="A126" s="2">
+        <v>45755.43242371528</v>
+      </c>
+      <c r="B126" t="s">
+        <v>26</v>
+      </c>
+      <c r="C126" t="s">
+        <v>31</v>
+      </c>
+      <c r="D126" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="A127" s="2">
+        <v>45755.44526734954</v>
+      </c>
+      <c r="B127" t="s">
+        <v>27</v>
+      </c>
+      <c r="C127" t="s">
+        <v>32</v>
+      </c>
+      <c r="D127" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128" s="2">
+        <v>45755.44527988426</v>
+      </c>
+      <c r="B128" t="s">
+        <v>28</v>
+      </c>
+      <c r="C128" t="s">
+        <v>32</v>
+      </c>
+      <c r="D128" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" s="2">
+        <v>45757.91495641533</v>
+      </c>
+      <c r="B129" t="s">
+        <v>29</v>
+      </c>
+      <c r="C129" t="s">
+        <v>33</v>
+      </c>
+      <c r="D129" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>